<commit_message>
se pushea cambios en casos de prueba
</commit_message>
<xml_diff>
--- a/Casos de Uso/Listado de Casos de Usos - 2019-02-08.xlsx
+++ b/Casos de Uso/Listado de Casos de Usos - 2019-02-08.xlsx
@@ -1,23 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\pablo\Desktop\irsaanfler\Casos de Uso\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Casos de Uso" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Casos de Prueba" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
+    <sheet name="Casos de Prueba" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">'Casos de Uso'!$1:$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">'Casos de Uso'!$1:$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0" vbProcedure="false">'Casos de Uso'!$1:$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0" vbProcedure="false">'Casos de Uso'!$1:$1</definedName>
+    <definedName name="Print_Titles_0" localSheetId="0">'Casos de Uso'!$1:$1</definedName>
+    <definedName name="Print_Titles_0_0" localSheetId="0">'Casos de Uso'!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$1:$1</definedName>
   </definedNames>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -27,421 +30,403 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="128">
-  <si>
-    <t xml:space="preserve">Caso de Uso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Título</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Módulo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Actor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CU G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CU D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ingresar al Sistema</t>
-  </si>
-  <si>
-    <t xml:space="preserve">General</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Salir del Sistema</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Registro de Auditoría</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crear Categoria de Archivos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Biblioteca Digital</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modificar Categoría de Archivos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deshabilitar Categoría de Archivos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crear Areas Responsables</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modificar Areas Responsables</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crear Centro de Costos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modificar Centro de Costos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deshabilitar Centro de Costos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crear Estudio Jurídico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modificar Estudio Jurídico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deshabilitar Estudio Jurídico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crear Etapa de Proceso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modificar Etapa de Proceso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deshabilitar Etapa de Proceso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crear Categoría de Aging</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modificar Categoría de Aging</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deshabilitar Categoría de Aging</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crear Inmueble</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modificar Inmueble</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deshabilitar Inmueble</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="128">
+  <si>
+    <t>Caso de Uso</t>
+  </si>
+  <si>
+    <t>Título</t>
+  </si>
+  <si>
+    <t>Módulo</t>
+  </si>
+  <si>
+    <t>Actor</t>
+  </si>
+  <si>
+    <t>CU G</t>
+  </si>
+  <si>
+    <t>CU D</t>
+  </si>
+  <si>
+    <t>CP</t>
+  </si>
+  <si>
+    <t>Ingresar al Sistema</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Salir del Sistema</t>
+  </si>
+  <si>
+    <t>Registro de Auditoría</t>
+  </si>
+  <si>
+    <t>Crear Categoria de Archivos</t>
+  </si>
+  <si>
+    <t>Biblioteca Digital</t>
+  </si>
+  <si>
+    <t>Modificar Categoría de Archivos</t>
+  </si>
+  <si>
+    <t>Deshabilitar Categoría de Archivos</t>
+  </si>
+  <si>
+    <t>Crear Areas Responsables</t>
+  </si>
+  <si>
+    <t>Modificar Areas Responsables</t>
+  </si>
+  <si>
+    <t>Crear Centro de Costos</t>
+  </si>
+  <si>
+    <t>Modificar Centro de Costos</t>
+  </si>
+  <si>
+    <t>Deshabilitar Centro de Costos</t>
+  </si>
+  <si>
+    <t>Crear Estudio Jurídico</t>
+  </si>
+  <si>
+    <t>Modificar Estudio Jurídico</t>
+  </si>
+  <si>
+    <t>Deshabilitar Estudio Jurídico</t>
+  </si>
+  <si>
+    <t>Crear Etapa de Proceso</t>
+  </si>
+  <si>
+    <t>Modificar Etapa de Proceso</t>
+  </si>
+  <si>
+    <t>Deshabilitar Etapa de Proceso</t>
+  </si>
+  <si>
+    <t>Crear Categoría de Aging</t>
+  </si>
+  <si>
+    <t>Modificar Categoría de Aging</t>
+  </si>
+  <si>
+    <t>Deshabilitar Categoría de Aging</t>
+  </si>
+  <si>
+    <t>Crear Inmueble</t>
+  </si>
+  <si>
+    <t>Modificar Inmueble</t>
+  </si>
+  <si>
+    <t>Deshabilitar Inmueble</t>
   </si>
   <si>
     <t xml:space="preserve">Crear Jurisdicción </t>
   </si>
   <si>
-    <t xml:space="preserve">Modificar Jurisdiccion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestionar Fuero</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crear Póliza</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modificar Póliza</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deshabilitar Póliza</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crear Parte de Juicio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modificar Parte de Juicio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deshabilitar Parte de Juicio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crear Tipo de Proceso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modificar Tipo de Proceso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deshabilitar Tipo de Proceso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crear Expediente Judicial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Expedientes Judiciales</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modificar Cabecera Expediente Judicial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ver Listados</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Terminar Expediente Judicial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reactivar Expediente Judicial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Archivar Expediente Judicial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Desarchivar Expediente Judicial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crear Directorio de Archivos en Expediente Judicial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Renombrar Directorio de Expediente Judicial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eliminar Directorio de Expediente Judicial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agregar Archivo a Expediente Judicial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Remover Archivo de Expediente Judicial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crear Consulta en Expediente Judicial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Responder Consulta en Expediente Judicial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Finalizar Consulta en Expediente Judicial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Registrar Acción Judicial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cargar Evento en Calendario de Expediente Judicial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modificar Evento en Calendario de Expediente Judicial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eliminar Evento de Calendario de Expediente Judicial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crear Esquela de Solicitud de Gastos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modificar Esquela de Solicitud de Gastos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aprobar Esquela de Solicitud de Gastos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notificar a Usuario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crear Persona</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sociedades y Agenda Societaria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modificar Persona</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eliminar Persona</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crear Sociedad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modificar Sociedad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eliminar Sociedad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Establecer Composicion Societaria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Establecer Composicion de Directorio</t>
+    <t>Modificar Jurisdiccion</t>
+  </si>
+  <si>
+    <t>Gestionar Fuero</t>
+  </si>
+  <si>
+    <t>Crear Póliza</t>
+  </si>
+  <si>
+    <t>Modificar Póliza</t>
+  </si>
+  <si>
+    <t>Deshabilitar Póliza</t>
+  </si>
+  <si>
+    <t>Crear Parte de Juicio</t>
+  </si>
+  <si>
+    <t>Modificar Parte de Juicio</t>
+  </si>
+  <si>
+    <t>Deshabilitar Parte de Juicio</t>
+  </si>
+  <si>
+    <t>Crear Tipo de Proceso</t>
+  </si>
+  <si>
+    <t>Modificar Tipo de Proceso</t>
+  </si>
+  <si>
+    <t>Deshabilitar Tipo de Proceso</t>
+  </si>
+  <si>
+    <t>Crear Expediente Judicial</t>
+  </si>
+  <si>
+    <t>Expedientes Judiciales</t>
+  </si>
+  <si>
+    <t>Modificar Cabecera Expediente Judicial</t>
+  </si>
+  <si>
+    <t>Ver Listados</t>
+  </si>
+  <si>
+    <t>Terminar Expediente Judicial</t>
+  </si>
+  <si>
+    <t>Reactivar Expediente Judicial</t>
+  </si>
+  <si>
+    <t>Archivar Expediente Judicial</t>
+  </si>
+  <si>
+    <t>Desarchivar Expediente Judicial</t>
+  </si>
+  <si>
+    <t>Crear Directorio de Archivos en Expediente Judicial</t>
+  </si>
+  <si>
+    <t>Renombrar Directorio de Expediente Judicial</t>
+  </si>
+  <si>
+    <t>Eliminar Directorio de Expediente Judicial</t>
+  </si>
+  <si>
+    <t>Agregar Archivo a Expediente Judicial</t>
+  </si>
+  <si>
+    <t>Remover Archivo de Expediente Judicial</t>
+  </si>
+  <si>
+    <t>Crear Consulta en Expediente Judicial</t>
+  </si>
+  <si>
+    <t>Responder Consulta en Expediente Judicial</t>
+  </si>
+  <si>
+    <t>Finalizar Consulta en Expediente Judicial</t>
+  </si>
+  <si>
+    <t>Registrar Acción Judicial</t>
+  </si>
+  <si>
+    <t>Cargar Evento en Calendario de Expediente Judicial</t>
+  </si>
+  <si>
+    <t>Modificar Evento en Calendario de Expediente Judicial</t>
+  </si>
+  <si>
+    <t>Eliminar Evento de Calendario de Expediente Judicial</t>
+  </si>
+  <si>
+    <t>Crear Esquela de Solicitud de Gastos</t>
+  </si>
+  <si>
+    <t>Modificar Esquela de Solicitud de Gastos</t>
+  </si>
+  <si>
+    <t>Aprobar Esquela de Solicitud de Gastos</t>
+  </si>
+  <si>
+    <t>Notificar a Usuario</t>
+  </si>
+  <si>
+    <t>Crear Persona</t>
+  </si>
+  <si>
+    <t>Sociedades y Agenda Societaria</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Modificar Persona</t>
+  </si>
+  <si>
+    <t>Eliminar Persona</t>
+  </si>
+  <si>
+    <t>Crear Sociedad</t>
+  </si>
+  <si>
+    <t>Modificar Sociedad</t>
+  </si>
+  <si>
+    <t>Eliminar Sociedad</t>
+  </si>
+  <si>
+    <t>Establecer Composicion Societaria</t>
+  </si>
+  <si>
+    <t>Establecer Composicion de Directorio</t>
   </si>
   <si>
     <t xml:space="preserve">Crear Cargo </t>
   </si>
   <si>
-    <t xml:space="preserve">Modificar Cargo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eliminar Cargo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crear Evento en Calendario Sociedad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modificar Evento en Calendario Sociedad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eliminar Evento de Calendario Sociedad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agregar Archivo a Biblioteca Digital</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eliminar Archivo de Biblioteca Digital</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crear Directorio en Biblioteca Digital</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Renombrar Directorio de Biblioteca Digital</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eliminar Directorio de Biblioteca Digital</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Buscar Archivos en Biblioteca Digital</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Consumir Archivos de Biblioteca Digital</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asociar Archivos de Biblioteca Digital a Expediente Judicial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crear Modelo de Acta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Actas Societarias y Gestión Documental</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modificar Modelo de Acta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eliminar Modelo de Acta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crear Solicitud de Acta Societaria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crear Versión de Acta Societaria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crear Revisión de Acta Societaria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aprobar Acta Societaria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Importar Honorarios</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crear Hito de Análisis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reportes e Informes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modificar Hito de Análisis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Generar Reporte de Auditores</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Generar Base Legales</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Generar Reporte a Medida</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Generar Reporte de Auditores Masivo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crear Apoderado de Sociedad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crear Categoria de Apoderado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eliminar Categoría de Apoderado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eliminar Apoderado de Sociedad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crear Lógica de Autorización de Apoderados</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eliminar Lógica de Autorización de Apoderados</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Buscar Apoderados por Monto a Autorizar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crear Perfil de Tareas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modificar Perfil de Tareas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eliminar Perfil de Tareas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crear Usuario Local</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modificar Usuario Local</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deshabilitar Usuario Local</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crear Usuario LDAP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ver Registros de Auditoría</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Auditoría del Sistema</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Buscar Elemento</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crear Grupo de Gráficos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modificar Grupo de Gráficos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eliminar Grupo de Gráficos</t>
+    <t>Modificar Cargo</t>
+  </si>
+  <si>
+    <t>Eliminar Cargo</t>
+  </si>
+  <si>
+    <t>Crear Evento en Calendario Sociedad</t>
+  </si>
+  <si>
+    <t>Modificar Evento en Calendario Sociedad</t>
+  </si>
+  <si>
+    <t>Eliminar Evento de Calendario Sociedad</t>
+  </si>
+  <si>
+    <t>Agregar Archivo a Biblioteca Digital</t>
+  </si>
+  <si>
+    <t>Eliminar Archivo de Biblioteca Digital</t>
+  </si>
+  <si>
+    <t>Crear Directorio en Biblioteca Digital</t>
+  </si>
+  <si>
+    <t>Renombrar Directorio de Biblioteca Digital</t>
+  </si>
+  <si>
+    <t>Eliminar Directorio de Biblioteca Digital</t>
+  </si>
+  <si>
+    <t>Buscar Archivos en Biblioteca Digital</t>
+  </si>
+  <si>
+    <t>Consumir Archivos de Biblioteca Digital</t>
+  </si>
+  <si>
+    <t>Asociar Archivos de Biblioteca Digital a Expediente Judicial</t>
+  </si>
+  <si>
+    <t>Crear Modelo de Acta</t>
+  </si>
+  <si>
+    <t>Actas Societarias y Gestión Documental</t>
+  </si>
+  <si>
+    <t>Modificar Modelo de Acta</t>
+  </si>
+  <si>
+    <t>Eliminar Modelo de Acta</t>
+  </si>
+  <si>
+    <t>Crear Solicitud de Acta Societaria</t>
+  </si>
+  <si>
+    <t>Crear Versión de Acta Societaria</t>
+  </si>
+  <si>
+    <t>Crear Revisión de Acta Societaria</t>
+  </si>
+  <si>
+    <t>Aprobar Acta Societaria</t>
+  </si>
+  <si>
+    <t>Importar Honorarios</t>
+  </si>
+  <si>
+    <t>Crear Hito de Análisis</t>
+  </si>
+  <si>
+    <t>Reportes e Informes</t>
+  </si>
+  <si>
+    <t>Modificar Hito de Análisis</t>
+  </si>
+  <si>
+    <t>Generar Reporte de Auditores</t>
+  </si>
+  <si>
+    <t>Generar Base Legales</t>
+  </si>
+  <si>
+    <t>Generar Reporte a Medida</t>
+  </si>
+  <si>
+    <t>Generar Reporte de Auditores Masivo</t>
+  </si>
+  <si>
+    <t>Crear Apoderado de Sociedad</t>
+  </si>
+  <si>
+    <t>Crear Categoria de Apoderado</t>
+  </si>
+  <si>
+    <t>Eliminar Categoría de Apoderado</t>
+  </si>
+  <si>
+    <t>Eliminar Apoderado de Sociedad</t>
+  </si>
+  <si>
+    <t>Crear Lógica de Autorización de Apoderados</t>
+  </si>
+  <si>
+    <t>Eliminar Lógica de Autorización de Apoderados</t>
+  </si>
+  <si>
+    <t>Buscar Apoderados por Monto a Autorizar</t>
+  </si>
+  <si>
+    <t>Crear Perfil de Tareas</t>
+  </si>
+  <si>
+    <t>Modificar Perfil de Tareas</t>
+  </si>
+  <si>
+    <t>Eliminar Perfil de Tareas</t>
+  </si>
+  <si>
+    <t>Crear Usuario Local</t>
+  </si>
+  <si>
+    <t>Modificar Usuario Local</t>
+  </si>
+  <si>
+    <t>Deshabilitar Usuario Local</t>
+  </si>
+  <si>
+    <t>Crear Usuario LDAP</t>
+  </si>
+  <si>
+    <t>Ver Registros de Auditoría</t>
+  </si>
+  <si>
+    <t>Auditoría del Sistema</t>
+  </si>
+  <si>
+    <t>Buscar Elemento</t>
+  </si>
+  <si>
+    <t>Crear Grupo de Gráficos</t>
+  </si>
+  <si>
+    <t>Modificar Grupo de Gráficos</t>
+  </si>
+  <si>
+    <t>Eliminar Grupo de Gráficos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="4">
@@ -465,88 +450,61 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -605,33 +563,310 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="true"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:G115"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D92" activeCellId="0" sqref="D92"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="53.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="36.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="5.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="10.65"/>
+    <col min="1" max="1" width="11.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="53.7109375" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="6" width="5.7109375" customWidth="1"/>
+    <col min="7" max="1025" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -654,8 +889,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="n">
+    <row r="2" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -669,8 +904,8 @@
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
+    <row r="3" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -684,8 +919,8 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
+    <row r="4" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -699,8 +934,8 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
+    <row r="5" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -714,8 +949,8 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
+    <row r="6" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -729,7 +964,7 @@
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="6" t="s">
         <v>14</v>
@@ -742,8 +977,8 @@
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="n">
+    <row r="8" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -757,8 +992,8 @@
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="n">
+    <row r="9" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -772,8 +1007,8 @@
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="n">
+    <row r="10" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
         <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -787,8 +1022,8 @@
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="n">
+    <row r="11" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -802,7 +1037,7 @@
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="6" t="s">
         <v>19</v>
@@ -815,8 +1050,8 @@
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
     </row>
-    <row r="13" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="n">
+    <row r="13" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
         <v>10</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -830,8 +1065,8 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="n">
+    <row r="14" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
         <v>11</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -845,7 +1080,7 @@
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="6" t="s">
         <v>22</v>
@@ -858,8 +1093,8 @@
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
     </row>
-    <row r="16" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="n">
+    <row r="16" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
         <v>12</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -873,8 +1108,8 @@
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="n">
+    <row r="17" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
         <v>13</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -888,7 +1123,7 @@
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="6" t="s">
         <v>25</v>
@@ -901,8 +1136,8 @@
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
     </row>
-    <row r="19" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="n">
+    <row r="19" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
         <v>14</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -916,8 +1151,8 @@
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="n">
+    <row r="20" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
         <v>15</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -931,7 +1166,7 @@
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="6" t="s">
         <v>28</v>
@@ -944,8 +1179,8 @@
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
     </row>
-    <row r="22" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="n">
+    <row r="22" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
         <v>16</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -959,8 +1194,8 @@
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="n">
+    <row r="23" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
         <v>17</v>
       </c>
       <c r="B23" s="4" t="s">
@@ -974,7 +1209,7 @@
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="6" t="s">
         <v>31</v>
@@ -987,8 +1222,8 @@
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
     </row>
-    <row r="25" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="n">
+    <row r="25" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
         <v>18</v>
       </c>
       <c r="B25" s="4" t="s">
@@ -1002,8 +1237,8 @@
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3" t="n">
+    <row r="26" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
         <v>19</v>
       </c>
       <c r="B26" s="4" t="s">
@@ -1017,8 +1252,8 @@
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3" t="n">
+    <row r="27" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
         <v>191</v>
       </c>
       <c r="B27" s="4" t="s">
@@ -1032,8 +1267,8 @@
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3" t="n">
+    <row r="28" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
         <v>20</v>
       </c>
       <c r="B28" s="4" t="s">
@@ -1047,8 +1282,8 @@
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
     </row>
-    <row r="29" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3" t="n">
+    <row r="29" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
         <v>21</v>
       </c>
       <c r="B29" s="4" t="s">
@@ -1062,7 +1297,7 @@
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
     </row>
-    <row r="30" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="6" t="s">
         <v>37</v>
@@ -1075,8 +1310,8 @@
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
     </row>
-    <row r="31" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3" t="n">
+    <row r="31" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
         <v>22</v>
       </c>
       <c r="B31" s="4" t="s">
@@ -1090,8 +1325,8 @@
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
     </row>
-    <row r="32" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="3" t="n">
+    <row r="32" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
         <v>23</v>
       </c>
       <c r="B32" s="4" t="s">
@@ -1105,7 +1340,7 @@
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
     </row>
-    <row r="33" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="6" t="s">
         <v>40</v>
@@ -1118,8 +1353,8 @@
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
     </row>
-    <row r="34" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="3" t="n">
+    <row r="34" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
         <v>24</v>
       </c>
       <c r="B34" s="4" t="s">
@@ -1133,8 +1368,8 @@
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
     </row>
-    <row r="35" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="3" t="n">
+    <row r="35" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
         <v>25</v>
       </c>
       <c r="B35" s="4" t="s">
@@ -1148,7 +1383,7 @@
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
     </row>
-    <row r="36" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" s="6" t="s">
         <v>43</v>
@@ -1161,8 +1396,8 @@
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
     </row>
-    <row r="37" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="3" t="n">
+    <row r="37" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
         <v>26</v>
       </c>
       <c r="B37" s="4" t="s">
@@ -1176,8 +1411,8 @@
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
     </row>
-    <row r="38" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="3" t="n">
+    <row r="38" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
         <v>27</v>
       </c>
       <c r="B38" s="4" t="s">
@@ -1191,7 +1426,7 @@
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
     </row>
-    <row r="39" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
       <c r="B39" s="6" t="s">
         <v>47</v>
@@ -1204,8 +1439,8 @@
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
     </row>
-    <row r="40" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="3" t="n">
+    <row r="40" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
         <v>28</v>
       </c>
       <c r="B40" s="4" t="s">
@@ -1219,8 +1454,8 @@
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
     </row>
-    <row r="41" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="3" t="n">
+    <row r="41" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
         <v>29</v>
       </c>
       <c r="B41" s="4" t="s">
@@ -1234,8 +1469,8 @@
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
     </row>
-    <row r="42" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="3" t="n">
+    <row r="42" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="3">
         <v>30</v>
       </c>
       <c r="B42" s="4" t="s">
@@ -1249,8 +1484,8 @@
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
     </row>
-    <row r="43" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="3" t="n">
+    <row r="43" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
         <v>31</v>
       </c>
       <c r="B43" s="4" t="s">
@@ -1264,8 +1499,8 @@
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
     </row>
-    <row r="44" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="3" t="n">
+    <row r="44" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="3">
         <v>32</v>
       </c>
       <c r="B44" s="4" t="s">
@@ -1279,8 +1514,8 @@
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
     </row>
-    <row r="45" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="3" t="n">
+    <row r="45" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="3">
         <v>33</v>
       </c>
       <c r="B45" s="4" t="s">
@@ -1294,8 +1529,8 @@
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
     </row>
-    <row r="46" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="3" t="n">
+    <row r="46" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="3">
         <v>34</v>
       </c>
       <c r="B46" s="4" t="s">
@@ -1309,8 +1544,8 @@
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
     </row>
-    <row r="47" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="3" t="n">
+    <row r="47" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="3">
         <v>35</v>
       </c>
       <c r="B47" s="4" t="s">
@@ -1324,8 +1559,8 @@
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
     </row>
-    <row r="48" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="3" t="n">
+    <row r="48" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="3">
         <v>36</v>
       </c>
       <c r="B48" s="4" t="s">
@@ -1339,8 +1574,8 @@
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
     </row>
-    <row r="49" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="3" t="n">
+    <row r="49" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3">
         <v>37</v>
       </c>
       <c r="B49" s="4" t="s">
@@ -1354,8 +1589,8 @@
       <c r="F49" s="4"/>
       <c r="G49" s="4"/>
     </row>
-    <row r="50" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="3" t="n">
+    <row r="50" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="3">
         <v>38</v>
       </c>
       <c r="B50" s="4" t="s">
@@ -1369,8 +1604,8 @@
       <c r="F50" s="4"/>
       <c r="G50" s="4"/>
     </row>
-    <row r="51" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="3" t="n">
+    <row r="51" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="3">
         <v>39</v>
       </c>
       <c r="B51" s="4" t="s">
@@ -1384,8 +1619,8 @@
       <c r="F51" s="4"/>
       <c r="G51" s="4"/>
     </row>
-    <row r="52" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="3" t="n">
+    <row r="52" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="3">
         <v>40</v>
       </c>
       <c r="B52" s="4" t="s">
@@ -1399,8 +1634,8 @@
       <c r="F52" s="4"/>
       <c r="G52" s="4"/>
     </row>
-    <row r="53" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="3" t="n">
+    <row r="53" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="3">
         <v>41</v>
       </c>
       <c r="B53" s="4" t="s">
@@ -1414,8 +1649,8 @@
       <c r="F53" s="4"/>
       <c r="G53" s="4"/>
     </row>
-    <row r="54" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="3" t="n">
+    <row r="54" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="3">
         <v>42</v>
       </c>
       <c r="B54" s="4" t="s">
@@ -1429,7 +1664,7 @@
       <c r="F54" s="4"/>
       <c r="G54" s="4"/>
     </row>
-    <row r="55" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="55" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5"/>
       <c r="B55" s="6" t="s">
         <v>63</v>
@@ -1442,8 +1677,8 @@
       <c r="F55" s="6"/>
       <c r="G55" s="6"/>
     </row>
-    <row r="56" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="3" t="n">
+    <row r="56" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="3">
         <v>43</v>
       </c>
       <c r="B56" s="4" t="s">
@@ -1457,8 +1692,8 @@
       <c r="F56" s="4"/>
       <c r="G56" s="4"/>
     </row>
-    <row r="57" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="3" t="n">
+    <row r="57" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="3">
         <v>44</v>
       </c>
       <c r="B57" s="4" t="s">
@@ -1472,8 +1707,8 @@
       <c r="F57" s="4"/>
       <c r="G57" s="4"/>
     </row>
-    <row r="58" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="3" t="n">
+    <row r="58" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="3">
         <v>45</v>
       </c>
       <c r="B58" s="4" t="s">
@@ -1487,8 +1722,8 @@
       <c r="F58" s="4"/>
       <c r="G58" s="4"/>
     </row>
-    <row r="59" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="3" t="n">
+    <row r="59" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="3">
         <v>46</v>
       </c>
       <c r="B59" s="4" t="s">
@@ -1502,8 +1737,8 @@
       <c r="F59" s="4"/>
       <c r="G59" s="4"/>
     </row>
-    <row r="60" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="3" t="n">
+    <row r="60" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="3">
         <v>47</v>
       </c>
       <c r="B60" s="4" t="s">
@@ -1519,8 +1754,8 @@
       <c r="F60" s="4"/>
       <c r="G60" s="4"/>
     </row>
-    <row r="61" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="3" t="n">
+    <row r="61" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="3">
         <v>48</v>
       </c>
       <c r="B61" s="4" t="s">
@@ -1536,7 +1771,7 @@
       <c r="F61" s="4"/>
       <c r="G61" s="4"/>
     </row>
-    <row r="62" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="62" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="5"/>
       <c r="B62" s="6" t="s">
         <v>72</v>
@@ -1549,8 +1784,8 @@
       <c r="F62" s="6"/>
       <c r="G62" s="6"/>
     </row>
-    <row r="63" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="3" t="n">
+    <row r="63" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="3">
         <v>49</v>
       </c>
       <c r="B63" s="4" t="s">
@@ -1566,8 +1801,8 @@
       <c r="F63" s="4"/>
       <c r="G63" s="4"/>
     </row>
-    <row r="64" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="3" t="n">
+    <row r="64" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="3">
         <v>50</v>
       </c>
       <c r="B64" s="4" t="s">
@@ -1583,8 +1818,8 @@
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>
     </row>
-    <row r="65" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="3" t="n">
+    <row r="65" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="3">
         <v>51</v>
       </c>
       <c r="B65" s="4" t="s">
@@ -1600,8 +1835,8 @@
       <c r="F65" s="4"/>
       <c r="G65" s="4"/>
     </row>
-    <row r="66" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="3" t="n">
+    <row r="66" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="3">
         <v>52</v>
       </c>
       <c r="B66" s="4" t="s">
@@ -1617,8 +1852,8 @@
       <c r="F66" s="4"/>
       <c r="G66" s="4"/>
     </row>
-    <row r="67" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="3" t="n">
+    <row r="67" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="3">
         <v>53</v>
       </c>
       <c r="B67" s="4" t="s">
@@ -1634,8 +1869,8 @@
       <c r="F67" s="4"/>
       <c r="G67" s="4"/>
     </row>
-    <row r="68" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="3" t="n">
+    <row r="68" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="3">
         <v>54</v>
       </c>
       <c r="B68" s="4" t="s">
@@ -1651,8 +1886,8 @@
       <c r="F68" s="4"/>
       <c r="G68" s="4"/>
     </row>
-    <row r="69" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="3" t="n">
+    <row r="69" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="3">
         <v>55</v>
       </c>
       <c r="B69" s="4" t="s">
@@ -1668,8 +1903,8 @@
       <c r="F69" s="4"/>
       <c r="G69" s="4"/>
     </row>
-    <row r="70" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="3" t="n">
+    <row r="70" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="3">
         <v>56</v>
       </c>
       <c r="B70" s="4" t="s">
@@ -1685,8 +1920,8 @@
       <c r="F70" s="4"/>
       <c r="G70" s="4"/>
     </row>
-    <row r="71" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="3" t="n">
+    <row r="71" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="3">
         <v>57</v>
       </c>
       <c r="B71" s="4" t="s">
@@ -1700,8 +1935,8 @@
       <c r="F71" s="4"/>
       <c r="G71" s="4"/>
     </row>
-    <row r="72" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="3" t="n">
+    <row r="72" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="3">
         <v>58</v>
       </c>
       <c r="B72" s="4" t="s">
@@ -1715,7 +1950,7 @@
       <c r="F72" s="4"/>
       <c r="G72" s="4"/>
     </row>
-    <row r="73" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="73" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="5"/>
       <c r="B73" s="6" t="s">
         <v>83</v>
@@ -1728,8 +1963,8 @@
       <c r="F73" s="6"/>
       <c r="G73" s="6"/>
     </row>
-    <row r="74" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="3" t="n">
+    <row r="74" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="3">
         <v>62</v>
       </c>
       <c r="B74" s="4" t="s">
@@ -1743,8 +1978,8 @@
       <c r="F74" s="4"/>
       <c r="G74" s="4"/>
     </row>
-    <row r="75" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="3" t="n">
+    <row r="75" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="3">
         <v>63</v>
       </c>
       <c r="B75" s="4" t="s">
@@ -1758,8 +1993,8 @@
       <c r="F75" s="4"/>
       <c r="G75" s="4"/>
     </row>
-    <row r="76" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="3" t="n">
+    <row r="76" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="3">
         <v>59</v>
       </c>
       <c r="B76" s="4" t="s">
@@ -1773,8 +2008,8 @@
       <c r="F76" s="4"/>
       <c r="G76" s="4"/>
     </row>
-    <row r="77" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="3" t="n">
+    <row r="77" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="3">
         <v>60</v>
       </c>
       <c r="B77" s="4" t="s">
@@ -1788,8 +2023,8 @@
       <c r="F77" s="4"/>
       <c r="G77" s="4"/>
     </row>
-    <row r="78" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="3" t="n">
+    <row r="78" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="3">
         <v>61</v>
       </c>
       <c r="B78" s="4" t="s">
@@ -1803,8 +2038,8 @@
       <c r="F78" s="4"/>
       <c r="G78" s="4"/>
     </row>
-    <row r="79" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="3" t="n">
+    <row r="79" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="3">
         <v>65</v>
       </c>
       <c r="B79" s="4" t="s">
@@ -1818,8 +2053,8 @@
       <c r="F79" s="4"/>
       <c r="G79" s="4"/>
     </row>
-    <row r="80" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="3" t="n">
+    <row r="80" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="3">
         <v>64</v>
       </c>
       <c r="B80" s="4" t="s">
@@ -1833,8 +2068,8 @@
       <c r="F80" s="4"/>
       <c r="G80" s="4"/>
     </row>
-    <row r="81" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A81" s="3" t="n">
+    <row r="81" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="3">
         <v>66</v>
       </c>
       <c r="B81" s="4" t="s">
@@ -1848,8 +2083,8 @@
       <c r="F81" s="4"/>
       <c r="G81" s="4"/>
     </row>
-    <row r="82" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A82" s="3" t="n">
+    <row r="82" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="3">
         <v>67</v>
       </c>
       <c r="B82" s="4" t="s">
@@ -1865,8 +2100,8 @@
       <c r="F82" s="4"/>
       <c r="G82" s="4"/>
     </row>
-    <row r="83" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A83" s="3" t="n">
+    <row r="83" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="3">
         <v>68</v>
       </c>
       <c r="B83" s="4" t="s">
@@ -1882,8 +2117,8 @@
       <c r="F83" s="4"/>
       <c r="G83" s="4"/>
     </row>
-    <row r="84" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A84" s="3" t="n">
+    <row r="84" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="3">
         <v>69</v>
       </c>
       <c r="B84" s="4" t="s">
@@ -1899,8 +2134,8 @@
       <c r="F84" s="4"/>
       <c r="G84" s="4"/>
     </row>
-    <row r="85" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A85" s="3" t="n">
+    <row r="85" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="3">
         <v>70</v>
       </c>
       <c r="B85" s="4" t="s">
@@ -1909,13 +2144,15 @@
       <c r="C85" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="D85" s="4"/>
+      <c r="D85" s="4" t="s">
+        <v>70</v>
+      </c>
       <c r="E85" s="4"/>
       <c r="F85" s="4"/>
       <c r="G85" s="4"/>
     </row>
-    <row r="86" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A86" s="3" t="n">
+    <row r="86" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="3">
         <v>71</v>
       </c>
       <c r="B86" s="4" t="s">
@@ -1929,8 +2166,8 @@
       <c r="F86" s="4"/>
       <c r="G86" s="4"/>
     </row>
-    <row r="87" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A87" s="3" t="n">
+    <row r="87" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="3">
         <v>72</v>
       </c>
       <c r="B87" s="4" t="s">
@@ -1944,8 +2181,8 @@
       <c r="F87" s="4"/>
       <c r="G87" s="4"/>
     </row>
-    <row r="88" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A88" s="3" t="n">
+    <row r="88" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="3">
         <v>73</v>
       </c>
       <c r="B88" s="4" t="s">
@@ -1959,8 +2196,8 @@
       <c r="F88" s="4"/>
       <c r="G88" s="4"/>
     </row>
-    <row r="89" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A89" s="3" t="n">
+    <row r="89" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="3">
         <v>74</v>
       </c>
       <c r="B89" s="4" t="s">
@@ -1974,8 +2211,8 @@
       <c r="F89" s="4"/>
       <c r="G89" s="4"/>
     </row>
-    <row r="90" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A90" s="3" t="n">
+    <row r="90" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="3">
         <v>75</v>
       </c>
       <c r="B90" s="4" t="s">
@@ -1989,8 +2226,8 @@
       <c r="F90" s="4"/>
       <c r="G90" s="4"/>
     </row>
-    <row r="91" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A91" s="3" t="n">
+    <row r="91" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="3">
         <v>76</v>
       </c>
       <c r="B91" s="4" t="s">
@@ -2004,8 +2241,8 @@
       <c r="F91" s="4"/>
       <c r="G91" s="4"/>
     </row>
-    <row r="92" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A92" s="3" t="n">
+    <row r="92" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="3">
         <v>77</v>
       </c>
       <c r="B92" s="4" t="s">
@@ -2019,8 +2256,8 @@
       <c r="F92" s="4"/>
       <c r="G92" s="4"/>
     </row>
-    <row r="93" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A93" s="3" t="n">
+    <row r="93" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="3">
         <v>78</v>
       </c>
       <c r="B93" s="4" t="s">
@@ -2034,8 +2271,8 @@
       <c r="F93" s="4"/>
       <c r="G93" s="4"/>
     </row>
-    <row r="94" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A94" s="3" t="n">
+    <row r="94" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="3">
         <v>79</v>
       </c>
       <c r="B94" s="4" t="s">
@@ -2049,8 +2286,8 @@
       <c r="F94" s="4"/>
       <c r="G94" s="4"/>
     </row>
-    <row r="95" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A95" s="3" t="n">
+    <row r="95" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="3">
         <v>80</v>
       </c>
       <c r="B95" s="4" t="s">
@@ -2064,7 +2301,7 @@
       <c r="F95" s="4"/>
       <c r="G95" s="4"/>
     </row>
-    <row r="96" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="96" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="7" t="s">
         <v>108</v>
@@ -2077,7 +2314,7 @@
       <c r="F96" s="7"/>
       <c r="G96" s="7"/>
     </row>
-    <row r="97" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="97" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="7" t="s">
         <v>109</v>
@@ -2090,7 +2327,7 @@
       <c r="F97" s="7"/>
       <c r="G97" s="7"/>
     </row>
-    <row r="98" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="98" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="7" t="s">
         <v>110</v>
@@ -2103,7 +2340,7 @@
       <c r="F98" s="7"/>
       <c r="G98" s="7"/>
     </row>
-    <row r="99" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="99" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="7" t="s">
         <v>111</v>
@@ -2116,7 +2353,7 @@
       <c r="F99" s="7"/>
       <c r="G99" s="7"/>
     </row>
-    <row r="100" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="100" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="7" t="s">
         <v>112</v>
@@ -2129,7 +2366,7 @@
       <c r="F100" s="7"/>
       <c r="G100" s="7"/>
     </row>
-    <row r="101" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="101" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
       <c r="B101" s="7" t="s">
         <v>113</v>
@@ -2142,7 +2379,7 @@
       <c r="F101" s="7"/>
       <c r="G101" s="7"/>
     </row>
-    <row r="102" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="102" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
       <c r="B102" s="7" t="s">
         <v>114</v>
@@ -2155,7 +2392,7 @@
       <c r="F102" s="7"/>
       <c r="G102" s="7"/>
     </row>
-    <row r="103" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="103" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2"/>
       <c r="B103" s="7" t="s">
         <v>115</v>
@@ -2168,7 +2405,7 @@
       <c r="F103" s="7"/>
       <c r="G103" s="7"/>
     </row>
-    <row r="104" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="104" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
       <c r="B104" s="7" t="s">
         <v>116</v>
@@ -2181,7 +2418,7 @@
       <c r="F104" s="7"/>
       <c r="G104" s="7"/>
     </row>
-    <row r="105" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="105" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2"/>
       <c r="B105" s="7" t="s">
         <v>117</v>
@@ -2194,7 +2431,7 @@
       <c r="F105" s="7"/>
       <c r="G105" s="7"/>
     </row>
-    <row r="106" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="106" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="2"/>
       <c r="B106" s="7" t="s">
         <v>118</v>
@@ -2207,7 +2444,7 @@
       <c r="F106" s="7"/>
       <c r="G106" s="7"/>
     </row>
-    <row r="107" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="107" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="2"/>
       <c r="B107" s="7" t="s">
         <v>119</v>
@@ -2220,7 +2457,7 @@
       <c r="F107" s="7"/>
       <c r="G107" s="7"/>
     </row>
-    <row r="108" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="108" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="2"/>
       <c r="B108" s="7" t="s">
         <v>120</v>
@@ -2233,7 +2470,7 @@
       <c r="F108" s="7"/>
       <c r="G108" s="7"/>
     </row>
-    <row r="109" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="109" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="2"/>
       <c r="B109" s="7" t="s">
         <v>121</v>
@@ -2246,7 +2483,7 @@
       <c r="F109" s="7"/>
       <c r="G109" s="7"/>
     </row>
-    <row r="110" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="110" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="2"/>
       <c r="B110" s="7" t="s">
         <v>122</v>
@@ -2259,7 +2496,7 @@
       <c r="F110" s="7"/>
       <c r="G110" s="7"/>
     </row>
-    <row r="111" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="111" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="2"/>
       <c r="B111" s="7" t="s">
         <v>124</v>
@@ -2272,7 +2509,7 @@
       <c r="F111" s="7"/>
       <c r="G111" s="7"/>
     </row>
-    <row r="112" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="112" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="2"/>
       <c r="B112" s="7" t="s">
         <v>125</v>
@@ -2285,7 +2522,7 @@
       <c r="F112" s="7"/>
       <c r="G112" s="7"/>
     </row>
-    <row r="113" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="113" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="2"/>
       <c r="B113" s="7" t="s">
         <v>126</v>
@@ -2298,7 +2535,7 @@
       <c r="F113" s="7"/>
       <c r="G113" s="7"/>
     </row>
-    <row r="114" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="114" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="2"/>
       <c r="B114" s="7" t="s">
         <v>127</v>
@@ -2311,7 +2548,7 @@
       <c r="F114" s="7"/>
       <c r="G114" s="7"/>
     </row>
-    <row r="115" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="115" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="3"/>
       <c r="B115" s="4"/>
       <c r="C115" s="4"/>
@@ -2321,38 +2558,25 @@
       <c r="G115" s="4"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.747916666666667" bottom="0.747916666666667" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="0" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.74791666666666701" bottom="0.74791666666666701" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.65"/>
+    <col min="1" max="1025" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
se adjuntan los nuevos archivos
</commit_message>
<xml_diff>
--- a/Casos de Uso/Listado de Casos de Usos - 2019-02-08.xlsx
+++ b/Casos de Uso/Listado de Casos de Usos - 2019-02-08.xlsx
@@ -18,6 +18,8 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">'Casos de Uso'!$1:$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0" vbProcedure="false">'Casos de Uso'!$1:$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0" vbProcedure="false">'Casos de Uso'!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0" vbProcedure="false">'Casos de Uso'!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0" vbProcedure="false">'Casos de Uso'!$1:$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="134">
   <si>
     <t xml:space="preserve">Caso de Uso</t>
   </si>
@@ -197,9 +199,6 @@
   </si>
   <si>
     <t xml:space="preserve">Renombrar Directorio de Expediente Judicial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A que se refiere con directorio, no veo la opcion renombrar</t>
   </si>
   <si>
     <t xml:space="preserve">Eliminar Directorio de Expediente Judicial</t>
@@ -654,8 +653,8 @@
   </sheetPr>
   <dimension ref="A1:G115"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D51" activeCellId="0" sqref="D51"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D76" activeCellId="0" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -708,7 +707,7 @@
       <c r="F2" s="4"/>
       <c r="G2" s="4" t="n">
         <f aca="false">COUNTIF(D2:D115, "x")</f>
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -728,7 +727,7 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4" t="n">
         <f aca="false">COUNTBLANK(D2:D95)</f>
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1418,9 +1417,7 @@
       <c r="C45" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D45" s="6" t="s">
-        <v>56</v>
-      </c>
+      <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
@@ -1430,14 +1427,12 @@
         <v>34</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D46" s="6" t="s">
-        <v>56</v>
-      </c>
+      <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
@@ -1447,7 +1442,7 @@
         <v>35</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>47</v>
@@ -1464,7 +1459,7 @@
         <v>36</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>47</v>
@@ -1481,13 +1476,13 @@
         <v>37</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>47</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
@@ -1498,13 +1493,13 @@
         <v>38</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
@@ -1515,13 +1510,13 @@
         <v>39</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
@@ -1532,7 +1527,7 @@
         <v>40</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>47</v>
@@ -1549,13 +1544,13 @@
         <v>41</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>47</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
@@ -1566,13 +1561,13 @@
         <v>42</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>47</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
@@ -1581,7 +1576,7 @@
     <row r="55" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="7"/>
       <c r="B55" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C55" s="8" t="s">
         <v>47</v>
@@ -1598,13 +1593,13 @@
         <v>43</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C56" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E56" s="6"/>
       <c r="F56" s="6"/>
@@ -1615,13 +1610,13 @@
         <v>44</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C57" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E57" s="6"/>
       <c r="F57" s="6"/>
@@ -1632,13 +1627,13 @@
         <v>45</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C58" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E58" s="6"/>
       <c r="F58" s="6"/>
@@ -1649,7 +1644,7 @@
         <v>46</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C59" s="6" t="s">
         <v>8</v>
@@ -1666,10 +1661,10 @@
         <v>47</v>
       </c>
       <c r="B60" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C60" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>74</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>9</v>
@@ -1683,10 +1678,10 @@
         <v>48</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D61" s="4" t="s">
         <v>9</v>
@@ -1698,10 +1693,10 @@
     <row r="62" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="7"/>
       <c r="B62" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D62" s="8" t="s">
         <v>9</v>
@@ -1715,10 +1710,10 @@
         <v>49</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>9</v>
@@ -1732,10 +1727,10 @@
         <v>50</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>9</v>
@@ -1749,10 +1744,10 @@
         <v>51</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D65" s="4" t="s">
         <v>9</v>
@@ -1766,10 +1761,10 @@
         <v>52</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D66" s="4" t="s">
         <v>9</v>
@@ -1783,10 +1778,10 @@
         <v>53</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D67" s="4" t="s">
         <v>9</v>
@@ -1800,10 +1795,10 @@
         <v>54</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D68" s="4" t="s">
         <v>9</v>
@@ -1817,10 +1812,10 @@
         <v>55</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D69" s="4" t="s">
         <v>9</v>
@@ -1834,10 +1829,10 @@
         <v>56</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D70" s="4" t="s">
         <v>9</v>
@@ -1851,12 +1846,14 @@
         <v>57</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D71" s="4"/>
+        <v>73</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
       <c r="G71" s="4"/>
@@ -1866,12 +1863,14 @@
         <v>58</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D72" s="4"/>
+        <v>73</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
       <c r="G72" s="4"/>
@@ -1879,10 +1878,10 @@
     <row r="73" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="7"/>
       <c r="B73" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D73" s="8" t="s">
         <v>9</v>
@@ -1896,12 +1895,14 @@
         <v>62</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C74" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D74" s="4"/>
+      <c r="D74" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="E74" s="4"/>
       <c r="F74" s="4"/>
       <c r="G74" s="4"/>
@@ -1911,12 +1912,14 @@
         <v>63</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D75" s="4"/>
+      <c r="D75" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="E75" s="4"/>
       <c r="F75" s="4"/>
       <c r="G75" s="4"/>
@@ -1926,7 +1929,7 @@
         <v>59</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C76" s="4" t="s">
         <v>14</v>
@@ -1941,7 +1944,7 @@
         <v>60</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>14</v>
@@ -1956,7 +1959,7 @@
         <v>61</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C78" s="4" t="s">
         <v>14</v>
@@ -1971,7 +1974,7 @@
         <v>65</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C79" s="4" t="s">
         <v>14</v>
@@ -1986,7 +1989,7 @@
         <v>64</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C80" s="4" t="s">
         <v>14</v>
@@ -2001,7 +2004,7 @@
         <v>66</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C81" s="4" t="s">
         <v>14</v>
@@ -2016,10 +2019,10 @@
         <v>67</v>
       </c>
       <c r="B82" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C82" s="4" t="s">
         <v>96</v>
-      </c>
-      <c r="C82" s="4" t="s">
-        <v>97</v>
       </c>
       <c r="D82" s="4" t="s">
         <v>9</v>
@@ -2033,10 +2036,10 @@
         <v>68</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D83" s="4" t="s">
         <v>9</v>
@@ -2050,10 +2053,10 @@
         <v>69</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D84" s="4" t="s">
         <v>9</v>
@@ -2067,10 +2070,10 @@
         <v>70</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D85" s="4" t="s">
         <v>9</v>
@@ -2084,13 +2087,13 @@
         <v>71</v>
       </c>
       <c r="B86" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D86" s="4" t="s">
         <v>101</v>
-      </c>
-      <c r="C86" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="D86" s="4" t="s">
-        <v>102</v>
       </c>
       <c r="E86" s="4"/>
       <c r="F86" s="4"/>
@@ -2101,13 +2104,13 @@
         <v>72</v>
       </c>
       <c r="B87" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D87" s="4" t="s">
         <v>103</v>
-      </c>
-      <c r="C87" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="D87" s="4" t="s">
-        <v>104</v>
       </c>
       <c r="E87" s="4"/>
       <c r="F87" s="4"/>
@@ -2118,13 +2121,13 @@
         <v>73</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E88" s="4"/>
       <c r="F88" s="4"/>
@@ -2135,10 +2138,10 @@
         <v>74</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D89" s="4" t="s">
         <v>9</v>
@@ -2152,10 +2155,10 @@
         <v>75</v>
       </c>
       <c r="B90" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C90" s="4" t="s">
         <v>107</v>
-      </c>
-      <c r="C90" s="4" t="s">
-        <v>108</v>
       </c>
       <c r="D90" s="4" t="s">
         <v>9</v>
@@ -2169,10 +2172,10 @@
         <v>76</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D91" s="4" t="s">
         <v>9</v>
@@ -2186,13 +2189,13 @@
         <v>77</v>
       </c>
       <c r="B92" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D92" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="C92" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="D92" s="4" t="s">
-        <v>111</v>
       </c>
       <c r="E92" s="4"/>
       <c r="F92" s="4"/>
@@ -2203,10 +2206,10 @@
         <v>78</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D93" s="4" t="s">
         <v>9</v>
@@ -2220,10 +2223,10 @@
         <v>79</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D94" s="4" t="s">
         <v>9</v>
@@ -2237,10 +2240,10 @@
         <v>80</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D95" s="4" t="s">
         <v>9</v>
@@ -2252,10 +2255,10 @@
     <row r="96" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="2"/>
       <c r="B96" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D96" s="9"/>
       <c r="E96" s="9"/>
@@ -2265,10 +2268,10 @@
     <row r="97" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="2"/>
       <c r="B97" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C97" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D97" s="9"/>
       <c r="E97" s="9"/>
@@ -2278,10 +2281,10 @@
     <row r="98" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="2"/>
       <c r="B98" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C98" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D98" s="9"/>
       <c r="E98" s="9"/>
@@ -2291,10 +2294,10 @@
     <row r="99" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="2"/>
       <c r="B99" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C99" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D99" s="9"/>
       <c r="E99" s="9"/>
@@ -2304,10 +2307,10 @@
     <row r="100" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="2"/>
       <c r="B100" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C100" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D100" s="9"/>
       <c r="E100" s="9"/>
@@ -2317,10 +2320,10 @@
     <row r="101" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="2"/>
       <c r="B101" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C101" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D101" s="9"/>
       <c r="E101" s="9"/>
@@ -2330,10 +2333,10 @@
     <row r="102" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="2"/>
       <c r="B102" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C102" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D102" s="9"/>
       <c r="E102" s="9"/>
@@ -2343,7 +2346,7 @@
     <row r="103" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="2"/>
       <c r="B103" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C103" s="9" t="s">
         <v>8</v>
@@ -2356,7 +2359,7 @@
     <row r="104" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="2"/>
       <c r="B104" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C104" s="9" t="s">
         <v>8</v>
@@ -2369,7 +2372,7 @@
     <row r="105" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="2"/>
       <c r="B105" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C105" s="9" t="s">
         <v>8</v>
@@ -2382,7 +2385,7 @@
     <row r="106" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="2"/>
       <c r="B106" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C106" s="9" t="s">
         <v>8</v>
@@ -2395,7 +2398,7 @@
     <row r="107" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="2"/>
       <c r="B107" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C107" s="9" t="s">
         <v>8</v>
@@ -2408,7 +2411,7 @@
     <row r="108" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="2"/>
       <c r="B108" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C108" s="9" t="s">
         <v>8</v>
@@ -2421,7 +2424,7 @@
     <row r="109" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="2"/>
       <c r="B109" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C109" s="9" t="s">
         <v>8</v>
@@ -2434,10 +2437,10 @@
     <row r="110" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="2"/>
       <c r="B110" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C110" s="9" t="s">
         <v>129</v>
-      </c>
-      <c r="C110" s="9" t="s">
-        <v>130</v>
       </c>
       <c r="D110" s="9"/>
       <c r="E110" s="9"/>
@@ -2447,7 +2450,7 @@
     <row r="111" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="2"/>
       <c r="B111" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C111" s="9" t="s">
         <v>8</v>
@@ -2460,7 +2463,7 @@
     <row r="112" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="2"/>
       <c r="B112" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C112" s="9" t="s">
         <v>8</v>
@@ -2473,7 +2476,7 @@
     <row r="113" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="2"/>
       <c r="B113" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C113" s="9" t="s">
         <v>8</v>
@@ -2486,7 +2489,7 @@
     <row r="114" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="2"/>
       <c r="B114" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C114" s="9" t="s">
         <v>8</v>
@@ -2524,7 +2527,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E24" activeCellId="1" sqref="D51 E24"/>
+      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
se adjuntan los nuevos archivos con los fix solucionados al momento
</commit_message>
<xml_diff>
--- a/Casos de Uso/Listado de Casos de Usos - 2019-02-08.xlsx
+++ b/Casos de Uso/Listado de Casos de Usos - 2019-02-08.xlsx
@@ -21,6 +21,8 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0" vbProcedure="false">'Casos de Uso'!$1:$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0" vbProcedure="false">'Casos de Uso'!$1:$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0" vbProcedure="false">'Casos de Uso'!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0" vbProcedure="false">'Casos de Uso'!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0_0_0" vbProcedure="false">'Casos de Uso'!$1:$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="132">
   <si>
     <t xml:space="preserve">Caso de Uso</t>
   </si>
@@ -337,13 +339,7 @@
     <t xml:space="preserve">Crear Versión de Acta Societaria</t>
   </si>
   <si>
-    <t xml:space="preserve">Hay ticket</t>
-  </si>
-  <si>
     <t xml:space="preserve">Crear Revisión de Acta Societaria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El no poder editar no puedo cambiar el estado</t>
   </si>
   <si>
     <t xml:space="preserve">Aprobar Acta Societaria</t>
@@ -654,8 +650,8 @@
   </sheetPr>
   <dimension ref="A1:G115"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D49" activeCellId="0" sqref="D49"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D73" activeCellId="0" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -708,7 +704,7 @@
       <c r="F2" s="4"/>
       <c r="G2" s="4" t="n">
         <f aca="false">COUNTIF(D2:D115, "x")</f>
-        <v>78</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1555,7 +1551,7 @@
         <v>47</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>60</v>
+        <v>9</v>
       </c>
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
@@ -1572,7 +1568,7 @@
         <v>47</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>60</v>
+        <v>9</v>
       </c>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
@@ -1857,7 +1853,7 @@
         <v>73</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>60</v>
+        <v>9</v>
       </c>
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
@@ -1874,7 +1870,7 @@
         <v>73</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>60</v>
+        <v>9</v>
       </c>
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
@@ -2110,7 +2106,7 @@
         <v>96</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>101</v>
+        <v>9</v>
       </c>
       <c r="E86" s="4"/>
       <c r="F86" s="4"/>
@@ -2121,13 +2117,13 @@
         <v>72</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C87" s="4" t="s">
         <v>96</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>103</v>
+        <v>9</v>
       </c>
       <c r="E87" s="4"/>
       <c r="F87" s="4"/>
@@ -2138,13 +2134,13 @@
         <v>73</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C88" s="4" t="s">
         <v>96</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>103</v>
+        <v>9</v>
       </c>
       <c r="E88" s="4"/>
       <c r="F88" s="4"/>
@@ -2155,7 +2151,7 @@
         <v>74</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C89" s="4" t="s">
         <v>96</v>
@@ -2172,10 +2168,10 @@
         <v>75</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D90" s="4" t="s">
         <v>9</v>
@@ -2189,10 +2185,10 @@
         <v>76</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D91" s="4" t="s">
         <v>9</v>
@@ -2206,13 +2202,13 @@
         <v>77</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E92" s="4"/>
       <c r="F92" s="4"/>
@@ -2223,10 +2219,10 @@
         <v>78</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D93" s="4" t="s">
         <v>9</v>
@@ -2240,10 +2236,10 @@
         <v>79</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D94" s="4" t="s">
         <v>9</v>
@@ -2257,10 +2253,10 @@
         <v>80</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D95" s="4" t="s">
         <v>9</v>
@@ -2272,7 +2268,7 @@
     <row r="96" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="2"/>
       <c r="B96" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C96" s="9" t="s">
         <v>73</v>
@@ -2285,7 +2281,7 @@
     <row r="97" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="2"/>
       <c r="B97" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C97" s="9" t="s">
         <v>73</v>
@@ -2298,7 +2294,7 @@
     <row r="98" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="2"/>
       <c r="B98" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C98" s="9" t="s">
         <v>73</v>
@@ -2311,7 +2307,7 @@
     <row r="99" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="2"/>
       <c r="B99" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C99" s="9" t="s">
         <v>73</v>
@@ -2324,7 +2320,7 @@
     <row r="100" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="2"/>
       <c r="B100" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C100" s="9" t="s">
         <v>73</v>
@@ -2337,7 +2333,7 @@
     <row r="101" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="2"/>
       <c r="B101" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C101" s="9" t="s">
         <v>73</v>
@@ -2350,7 +2346,7 @@
     <row r="102" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="2"/>
       <c r="B102" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C102" s="9" t="s">
         <v>73</v>
@@ -2363,7 +2359,7 @@
     <row r="103" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="2"/>
       <c r="B103" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C103" s="9" t="s">
         <v>8</v>
@@ -2376,7 +2372,7 @@
     <row r="104" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="2"/>
       <c r="B104" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C104" s="9" t="s">
         <v>8</v>
@@ -2389,7 +2385,7 @@
     <row r="105" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="2"/>
       <c r="B105" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C105" s="9" t="s">
         <v>8</v>
@@ -2402,7 +2398,7 @@
     <row r="106" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="2"/>
       <c r="B106" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C106" s="9" t="s">
         <v>8</v>
@@ -2415,7 +2411,7 @@
     <row r="107" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="2"/>
       <c r="B107" s="9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C107" s="9" t="s">
         <v>8</v>
@@ -2428,7 +2424,7 @@
     <row r="108" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="2"/>
       <c r="B108" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C108" s="9" t="s">
         <v>8</v>
@@ -2441,7 +2437,7 @@
     <row r="109" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="2"/>
       <c r="B109" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C109" s="9" t="s">
         <v>8</v>
@@ -2454,10 +2450,10 @@
     <row r="110" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="2"/>
       <c r="B110" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C110" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D110" s="9"/>
       <c r="E110" s="9"/>
@@ -2467,7 +2463,7 @@
     <row r="111" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="2"/>
       <c r="B111" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C111" s="9" t="s">
         <v>8</v>
@@ -2480,7 +2476,7 @@
     <row r="112" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="2"/>
       <c r="B112" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C112" s="9" t="s">
         <v>8</v>
@@ -2493,7 +2489,7 @@
     <row r="113" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="2"/>
       <c r="B113" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C113" s="9" t="s">
         <v>8</v>
@@ -2506,7 +2502,7 @@
     <row r="114" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="2"/>
       <c r="B114" s="9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C114" s="9" t="s">
         <v>8</v>

</xml_diff>